<commit_message>
Test Plan with Scenarios
</commit_message>
<xml_diff>
--- a/BBlog _TestPlan.xlsx
+++ b/BBlog _TestPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSrinivasan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\bblog-api-test-automation-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B7BEF7-246A-453E-AF34-B092C834F612}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E059E53F-C667-4DD5-9A6C-22D309E20244}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA9A5D4F-F9E2-4ED8-A5D5-0AC6D4CA9506}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="303">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -2932,7 +2932,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8BC149-0BF0-4915-95D8-324D0594ACF7}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3704,7 +3706,9 @@
       <c r="J29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K29" s="10"/>
+      <c r="K29" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="L29" s="10"/>
     </row>
     <row r="30" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -3736,7 +3740,9 @@
       <c r="J30" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="K30" s="10"/>
+      <c r="K30" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="L30" s="10" t="s">
         <v>259</v>
       </c>
@@ -3818,7 +3824,9 @@
       <c r="J33" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="K33" s="15"/>
+      <c r="K33" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="L33" s="15"/>
     </row>
     <row r="34" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -3850,7 +3858,9 @@
       <c r="J34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K34" s="10"/>
+      <c r="K34" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="L34" s="10"/>
     </row>
     <row r="35" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -3882,7 +3892,9 @@
       <c r="J35" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K35" s="10"/>
+      <c r="K35" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="L35" s="10"/>
     </row>
     <row r="36" spans="1:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3914,7 +3926,9 @@
       <c r="J36" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="K36" s="25"/>
+      <c r="K36" s="25" t="s">
+        <v>93</v>
+      </c>
       <c r="L36" s="25"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>